<commit_message>
Tablas 8 y 9
</commit_message>
<xml_diff>
--- a/ENADEL 2023/Tablas/porcentajes.xlsx
+++ b/ENADEL 2023/Tablas/porcentajes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchile-my.sharepoint.com/personal/gocampo_fen_uchile_cl/Documents/Escritorio/Repositorios/ACNUR/ENADEL 2023/Tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="11_BA5482F5C8CC89882C3981443EAC11BCDFE98345" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEEAF9B7-9F22-4BA3-97F0-942FFC9F9FF7}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="11_BA5482F5C8CC89882C3981443EAC11BCDFE98345" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4457DBF3-2B61-4C81-AFBA-F7F0B292A8A2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pc_acteco" sheetId="1" r:id="rId1"/>
@@ -1689,10 +1689,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -2616,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F1048"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F968" sqref="F968"/>
     </sheetView>
   </sheetViews>
@@ -21634,7 +21630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -22684,12 +22682,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="65.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Tabla 10, 11 y 12
</commit_message>
<xml_diff>
--- a/ENADEL 2023/Tablas/porcentajes.xlsx
+++ b/ENADEL 2023/Tablas/porcentajes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchile-my.sharepoint.com/personal/gocampo_fen_uchile_cl/Documents/Escritorio/Repositorios/ACNUR/ENADEL 2023/Tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="11_BA5482F5C8CC89882C3981443EAC11BCDFE98345" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4457DBF3-2B61-4C81-AFBA-F7F0B292A8A2}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="11_BA5482F5C8CC89882C3981443EAC11BCDFE98345" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC7DF9A5-F018-4C06-B359-A4AFA695DE28}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pc_acteco" sheetId="1" r:id="rId1"/>
@@ -21630,13 +21630,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="52.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -22682,7 +22683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -24663,6 +24664,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="50.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Tablas 13, 14, 15 y 16
</commit_message>
<xml_diff>
--- a/ENADEL 2023/Tablas/porcentajes.xlsx
+++ b/ENADEL 2023/Tablas/porcentajes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchile-my.sharepoint.com/personal/gocampo_fen_uchile_cl/Documents/Escritorio/Repositorios/ACNUR/ENADEL 2023/Tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="11_BA5482F5C8CC89882C3981443EAC11BCDFE98345" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC7DF9A5-F018-4C06-B359-A4AFA695DE28}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="11_BA5482F5C8CC89882C3981443EAC11BCDFE98345" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6998498B-DC99-4BCA-9D47-25EB281A104A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="19" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pc_acteco" sheetId="1" r:id="rId1"/>
@@ -21630,7 +21630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -23349,7 +23349,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -23857,7 +23859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -25566,7 +25570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>